<commit_message>
Removed unused vs project files. Fixed method to return a XLOPer  to Excel
</commit_message>
<xml_diff>
--- a/TestXLL.xlsx
+++ b/TestXLL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>x</t>
   </si>
@@ -57,8 +57,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1308,7 +1310,7 @@
   <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1319,7 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>100</v>
       </c>
@@ -1325,7 +1327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -1337,414 +1339,443 @@
         <f ca="1">$B$1</f>
         <v>1</v>
       </c>
-      <c r="E2" t="e">
-        <f ca="1">_xll.MultiplicateArray(C2:D3)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <f t="array" aca="1" ref="E2:E18" ca="1">_xll.MultiplicateArray(C2:D18)</f>
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <f ca="1">_xll.MultiplicateArray(C2:D2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C55" ca="1" si="0">$A$1</f>
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D55" ca="1" si="1">$B$1</f>
-        <v>1</v>
-      </c>
-      <c r="E3" t="e">
-        <f ca="1">_xll.MultiplicateArray(C3:D4)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D3:D55" ca="1" si="0">$B$1</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f ca="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E4" t="e">
-        <f ca="1">_xll.MultiplicateArray(C4:D5)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <f ca="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E5" t="e">
-        <f ca="1">_xll.MultiplicateArray(C5:D6)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <f ca="1"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C6" ca="1" si="1">$A$1</f>
         <v>100</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E6" t="e">
-        <f ca="1">_xll.MultiplicateArray(C6:D7)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <f ca="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <f ca="1"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f ca="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C10" ca="1" si="2">$A$1</f>
         <v>100</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <f ca="1"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <f ca="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <f ca="1"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C14" ca="1" si="3">$A$1</f>
         <v>100</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <f ca="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <f ca="1"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <f ca="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C18" ca="1" si="4">$A$1</f>
         <v>100</v>
       </c>
       <c r="D18">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <f ca="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="D19">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="D20">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="D21">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C22" ca="1" si="5">$A$1</f>
         <v>100</v>
       </c>
       <c r="D22">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D23">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="D24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="D25">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C26" ca="1" si="6">$A$1</f>
         <v>100</v>
       </c>
       <c r="D26">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D27">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="D28">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29">
-        <f ca="1">$A$1</f>
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="D29">
         <f ca="1">$B$1</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C30" ca="1" si="7">$A$1</f>
         <v>100</v>
       </c>
       <c r="D30">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D31">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="D32">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1753,11 +1784,10 @@
         <v>32</v>
       </c>
       <c r="C33">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D33">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1766,11 +1796,11 @@
         <v>33</v>
       </c>
       <c r="C34">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C34" ca="1" si="8">$A$1</f>
         <v>100</v>
       </c>
       <c r="D34">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1779,11 +1809,10 @@
         <v>34</v>
       </c>
       <c r="C35">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="D35">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1792,11 +1821,10 @@
         <v>35</v>
       </c>
       <c r="C36">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="D36">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1805,11 +1833,10 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="D37">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1818,11 +1845,11 @@
         <v>37</v>
       </c>
       <c r="C38">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C38" ca="1" si="9">$A$1</f>
         <v>100</v>
       </c>
       <c r="D38">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1831,11 +1858,10 @@
         <v>38</v>
       </c>
       <c r="C39">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>128</v>
       </c>
       <c r="D39">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1844,11 +1870,10 @@
         <v>39</v>
       </c>
       <c r="C40">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="D40">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1857,11 +1882,10 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="D41">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1870,11 +1894,11 @@
         <v>41</v>
       </c>
       <c r="C42">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C42" ca="1" si="10">$A$1</f>
         <v>100</v>
       </c>
       <c r="D42">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1883,11 +1907,10 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="D43">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1896,11 +1919,10 @@
         <v>43</v>
       </c>
       <c r="C44">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>132</v>
       </c>
       <c r="D44">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1909,11 +1931,10 @@
         <v>44</v>
       </c>
       <c r="C45">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>133</v>
       </c>
       <c r="D45">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1922,11 +1943,11 @@
         <v>45</v>
       </c>
       <c r="C46">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C46" ca="1" si="11">$A$1</f>
         <v>100</v>
       </c>
       <c r="D46">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1935,11 +1956,10 @@
         <v>46</v>
       </c>
       <c r="C47">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="D47">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1948,11 +1968,10 @@
         <v>47</v>
       </c>
       <c r="C48">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="D48">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1961,11 +1980,10 @@
         <v>48</v>
       </c>
       <c r="C49">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>136</v>
       </c>
       <c r="D49">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1974,11 +1992,11 @@
         <v>49</v>
       </c>
       <c r="C50">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C50" ca="1" si="12">$A$1</f>
         <v>100</v>
       </c>
       <c r="D50">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -1987,11 +2005,10 @@
         <v>50</v>
       </c>
       <c r="C51">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>137</v>
       </c>
       <c r="D51">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2000,11 +2017,10 @@
         <v>51</v>
       </c>
       <c r="C52">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="D52">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2013,11 +2029,10 @@
         <v>52</v>
       </c>
       <c r="C53">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="D53">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2026,11 +2041,11 @@
         <v>53</v>
       </c>
       <c r="C54">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="C54" ca="1" si="13">$A$1</f>
         <v>100</v>
       </c>
       <c r="D54">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2039,11 +2054,10 @@
         <v>54</v>
       </c>
       <c r="C55">
-        <f t="shared" ca="1" si="0"/>
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="D55">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2051,8 +2065,8 @@
       <c r="B56" t="s">
         <v>0</v>
       </c>
-      <c r="C56" t="s">
-        <v>0</v>
+      <c r="C56">
+        <v>141</v>
       </c>
       <c r="D56" t="s">
         <v>0</v>
@@ -2068,8 +2082,8 @@
       <c r="B57" t="s">
         <v>0</v>
       </c>
-      <c r="C57" t="s">
-        <v>1</v>
+      <c r="C57">
+        <v>142</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
@@ -2083,6 +2097,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>